<commit_message>
feat: Enhance Payroll and Tax Management UI
- Updated PayrollProgressDialog to improve message display colors for errors and warnings.
- Refactored PayrollRunDetailsView to support dynamic payroll run selection and improved loading states.
- Integrated new API endpoint for fetching payroll run details and added error handling.
- Updated API_BASE_URL to point to the production server.
- Enhanced PayrollPage layout for better responsiveness and visual appeal.
- Revamped TaxPage to include detailed tax calculation parameters and improved tab navigation.
- Added loading indicators and error messages for better user experience in TaxPage.
- Introduced reusable components for displaying rate tables and card containers.
</commit_message>
<xml_diff>
--- a/src/assets/employee_import_template.xlsx
+++ b/src/assets/employee_import_template.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashley\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F3B3A9D-8C19-4DC4-BB65-EAFB59DD5FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="109">
   <si>
     <t>employee_number</t>
   </si>
@@ -124,10 +130,10 @@
     <t>is_helb_paying</t>
   </si>
   <si>
-    <t>benefits</t>
-  </si>
-  <si>
-    <t>extra_deductions</t>
+    <t>allowances_json</t>
+  </si>
+  <si>
+    <t>other_deductions_json</t>
   </si>
   <si>
     <t>paye_tax_exemption</t>
@@ -157,6 +163,42 @@
     <t>next_of_kin_phone</t>
   </si>
   <si>
+    <t>non_cash_benefits_json</t>
+  </si>
+  <si>
+    <t>helb_account_number</t>
+  </si>
+  <si>
+    <t>helb_monthly_deduction_amount</t>
+  </si>
+  <si>
+    <t>owner_occupied_interest_amount</t>
+  </si>
+  <si>
+    <t>pension_fund_contribution_amount</t>
+  </si>
+  <si>
+    <t>fbt_loan_type</t>
+  </si>
+  <si>
+    <t>fbt_loan_principal_amount</t>
+  </si>
+  <si>
+    <t>fbt_loan_interest_rate_charged</t>
+  </si>
+  <si>
+    <t>fbt_loan_start_date</t>
+  </si>
+  <si>
+    <t>fbt_loan_is_active</t>
+  </si>
+  <si>
+    <t>paye_exemption_certificate_number</t>
+  </si>
+  <si>
+    <t>disability_exemption_certificate_number</t>
+  </si>
+  <si>
     <t>EMP001</t>
   </si>
   <si>
@@ -181,18 +223,6 @@
     <t>Anne</t>
   </si>
   <si>
-    <t>john.doe@example.com</t>
-  </si>
-  <si>
-    <t>jane.smith@example.com</t>
-  </si>
-  <si>
-    <t>0712345678</t>
-  </si>
-  <si>
-    <t>0712345679</t>
-  </si>
-  <si>
     <t>National ID</t>
   </si>
   <si>
@@ -211,18 +241,6 @@
     <t>B987654321</t>
   </si>
   <si>
-    <t>123456</t>
-  </si>
-  <si>
-    <t>654321</t>
-  </si>
-  <si>
-    <t>1234567890</t>
-  </si>
-  <si>
-    <t>0987654321</t>
-  </si>
-  <si>
     <t>1990-01-01</t>
   </si>
   <si>
@@ -298,12 +316,6 @@
     <t>Mombasa</t>
   </si>
   <si>
-    <t>068</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
     <t>123 Main St, Nairobi</t>
   </si>
   <si>
@@ -316,12 +328,6 @@
     <t>P.O. Box 67890</t>
   </si>
   <si>
-    <t>00100</t>
-  </si>
-  <si>
-    <t>80100</t>
-  </si>
-  <si>
     <t>Alice Doe</t>
   </si>
   <si>
@@ -334,17 +340,20 @@
     <t>Brother</t>
   </si>
   <si>
-    <t>0723456789</t>
-  </si>
-  <si>
-    <t>0734567890</t>
+    <t>[{"type":"Housing","amount":5000},{"type":"Transport","amount":2000}]</t>
+  </si>
+  <si>
+    <t>ashleychiteri@gmail.com</t>
+  </si>
+  <si>
+    <t>punkzebra777@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -407,13 +416,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -451,7 +468,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -485,6 +502,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -519,9 +537,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -694,14 +713,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AU3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BG3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AV1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="BE9" sqref="BE9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.28515625" customWidth="1"/>
+    <col min="5" max="5" width="35.7109375" customWidth="1"/>
+    <col min="30" max="30" width="24.85546875" customWidth="1"/>
+    <col min="47" max="47" width="15.5703125" customWidth="1"/>
+    <col min="48" max="48" width="35.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:47">
+    <row r="1" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -843,106 +871,142 @@
       <c r="AU1" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="AV1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>58</v>
+      </c>
     </row>
-    <row r="2" spans="1:47">
+    <row r="2" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="E2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F2" t="s">
-        <v>57</v>
+        <v>107</v>
+      </c>
+      <c r="F2">
+        <v>712345678</v>
       </c>
       <c r="G2" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="H2" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="I2" t="s">
-        <v>63</v>
-      </c>
-      <c r="J2" t="s">
-        <v>65</v>
-      </c>
-      <c r="K2" t="s">
-        <v>67</v>
+        <v>71</v>
+      </c>
+      <c r="J2">
+        <v>123456</v>
+      </c>
+      <c r="K2">
+        <v>1234567890</v>
       </c>
       <c r="L2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="M2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="N2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="O2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="P2" t="b">
         <v>0</v>
       </c>
       <c r="Q2" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="R2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="S2" t="s">
+        <v>84</v>
+      </c>
+      <c r="T2" t="s">
+        <v>86</v>
+      </c>
+      <c r="U2" t="s">
+        <v>88</v>
+      </c>
+      <c r="V2" t="s">
         <v>80</v>
       </c>
-      <c r="T2" t="s">
-        <v>82</v>
-      </c>
-      <c r="U2" t="s">
-        <v>84</v>
-      </c>
-      <c r="V2" t="s">
-        <v>76</v>
-      </c>
       <c r="W2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="X2" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="Y2" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="AB2">
         <v>120000</v>
       </c>
       <c r="AC2" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="AD2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="AE2" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="AF2" t="s">
-        <v>92</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>94</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>57</v>
+        <v>96</v>
+      </c>
+      <c r="AG2">
+        <v>68</v>
+      </c>
+      <c r="AH2">
+        <v>1234567890</v>
+      </c>
+      <c r="AI2">
+        <v>712345678</v>
       </c>
       <c r="AJ2" t="b">
         <v>1</v>
@@ -960,15 +1024,15 @@
         <v>0</v>
       </c>
       <c r="AO2" t="s">
+        <v>98</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AQ2" t="s">
         <v>96</v>
       </c>
-      <c r="AP2" t="s">
-        <v>98</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>92</v>
-      </c>
-      <c r="AR2" t="s">
+      <c r="AR2">
         <v>100</v>
       </c>
       <c r="AS2" t="s">
@@ -977,109 +1041,145 @@
       <c r="AT2" t="s">
         <v>104</v>
       </c>
-      <c r="AU2" t="s">
+      <c r="AU2">
+        <v>723456789</v>
+      </c>
+      <c r="AV2" t="s">
         <v>106</v>
       </c>
+      <c r="AW2">
+        <v>0</v>
+      </c>
+      <c r="AX2">
+        <v>0</v>
+      </c>
+      <c r="AY2">
+        <v>0</v>
+      </c>
+      <c r="AZ2">
+        <v>0</v>
+      </c>
+      <c r="BA2">
+        <v>0</v>
+      </c>
+      <c r="BB2">
+        <v>0</v>
+      </c>
+      <c r="BC2">
+        <v>0</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE2" t="b">
+        <v>1</v>
+      </c>
+      <c r="BF2">
+        <v>0</v>
+      </c>
+      <c r="BG2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:47">
+    <row r="3" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="D3" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="E3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F3" t="s">
-        <v>58</v>
+        <v>108</v>
+      </c>
+      <c r="F3">
+        <v>712345679</v>
       </c>
       <c r="G3" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="H3" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="I3" t="s">
-        <v>64</v>
-      </c>
-      <c r="J3" t="s">
-        <v>66</v>
-      </c>
-      <c r="K3" t="s">
-        <v>68</v>
+        <v>72</v>
+      </c>
+      <c r="J3">
+        <v>654321</v>
+      </c>
+      <c r="K3">
+        <v>987654321</v>
       </c>
       <c r="L3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="M3" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="N3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="O3" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="P3" t="b">
         <v>1</v>
       </c>
       <c r="Q3" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="R3" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="S3" t="s">
+        <v>85</v>
+      </c>
+      <c r="T3" t="s">
+        <v>87</v>
+      </c>
+      <c r="U3" t="s">
+        <v>88</v>
+      </c>
+      <c r="V3" t="s">
         <v>81</v>
       </c>
-      <c r="T3" t="s">
-        <v>83</v>
-      </c>
-      <c r="U3" t="s">
-        <v>84</v>
-      </c>
-      <c r="V3" t="s">
-        <v>77</v>
-      </c>
       <c r="W3" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="X3" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="Y3" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="AB3">
         <v>150000</v>
       </c>
       <c r="AC3" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AD3" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="AE3" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="AF3" t="s">
-        <v>93</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>95</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>58</v>
+        <v>97</v>
+      </c>
+      <c r="AG3">
+        <v>100</v>
+      </c>
+      <c r="AH3">
+        <v>987654321</v>
+      </c>
+      <c r="AI3">
+        <v>712345679</v>
       </c>
       <c r="AJ3" t="b">
         <v>0</v>
@@ -1097,16 +1197,16 @@
         <v>1</v>
       </c>
       <c r="AO3" t="s">
+        <v>99</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>101</v>
+      </c>
+      <c r="AQ3" t="s">
         <v>97</v>
       </c>
-      <c r="AP3" t="s">
-        <v>99</v>
-      </c>
-      <c r="AQ3" t="s">
-        <v>93</v>
-      </c>
-      <c r="AR3" t="s">
-        <v>101</v>
+      <c r="AR3">
+        <v>80100</v>
       </c>
       <c r="AS3" t="s">
         <v>103</v>
@@ -1114,8 +1214,44 @@
       <c r="AT3" t="s">
         <v>105</v>
       </c>
-      <c r="AU3" t="s">
-        <v>107</v>
+      <c r="AU3">
+        <v>734567890</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>106</v>
+      </c>
+      <c r="AW3">
+        <v>0</v>
+      </c>
+      <c r="AX3">
+        <v>0</v>
+      </c>
+      <c r="AY3">
+        <v>0</v>
+      </c>
+      <c r="AZ3">
+        <v>0</v>
+      </c>
+      <c r="BA3">
+        <v>0</v>
+      </c>
+      <c r="BB3">
+        <v>0</v>
+      </c>
+      <c r="BC3">
+        <v>0</v>
+      </c>
+      <c r="BD3" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE3" t="b">
+        <v>1</v>
+      </c>
+      <c r="BF3">
+        <v>0</v>
+      </c>
+      <c r="BG3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>